<commit_message>
Actualizacion del porcentaje de avance del proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/MP/Gestión/MP-CP.xlsx
+++ b/Desarrollo/MP/Gestión/MP-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUZ ELENA\Downloads\Nueva carpeta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUZ ELENA\Documents\GitHub\Orangesoft\Desarrollo\MP\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD81FC-344C-4008-951A-B08F108E8B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEFBB1E-4E6E-4AA1-949E-12EE6F351DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1355,8 +1355,8 @@
   </sheetPr>
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1776,7 +1776,7 @@
         <v>44508</v>
       </c>
       <c r="H20" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>58</v>
@@ -1803,7 +1803,7 @@
         <v>44509</v>
       </c>
       <c r="H21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="65" t="s">
         <v>63</v>
@@ -1830,7 +1830,7 @@
         <v>44510</v>
       </c>
       <c r="H22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="66"/>
     </row>
@@ -1849,7 +1849,7 @@
         <v>44510</v>
       </c>
       <c r="H23" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="66"/>
     </row>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="I36" s="66"/>
     </row>
-    <row r="37" spans="1:9" ht="25.5">
+    <row r="37" spans="1:9" ht="14.25" customHeight="1">
       <c r="A37" s="11"/>
       <c r="B37" s="42" t="s">
         <v>91</v>
@@ -7239,7 +7239,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" ht="12.75">
       <c r="B5" s="61" t="s">
         <v>112</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" ht="12.75">
       <c r="B6" s="61" t="s">
         <v>114</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" ht="12.75">
       <c r="B7" s="61" t="s">
         <v>116</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" ht="12.75">
       <c r="B8" s="61" t="s">
         <v>118</v>
       </c>
@@ -7271,7 +7271,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" ht="12.75">
       <c r="B9" s="61" t="s">
         <v>120</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" ht="12.75">
       <c r="B10" s="61" t="s">
         <v>122</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" ht="12.75">
       <c r="B11" s="63" t="s">
         <v>123</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion porcentaje de avance del Cronograma del Proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/MP/Gestión/MP-CP.xlsx
+++ b/Desarrollo/MP/Gestión/MP-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUZ ELENA\Documents\GitHub\Orangesoft\Desarrollo\MP\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEFBB1E-4E6E-4AA1-949E-12EE6F351DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1465B14A-B362-49F1-8480-3D7ECE88C647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1355,8 +1355,8 @@
   </sheetPr>
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1874,7 +1874,7 @@
         <v>44523</v>
       </c>
       <c r="H24" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="65" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Actualizacion del porcentaje del cronograma del proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/MP/Gestión/MP-CP.xlsx
+++ b/Desarrollo/MP/Gestión/MP-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUZ ELENA\Documents\GitHub\Orangesoft\Desarrollo\MP\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1465B14A-B362-49F1-8480-3D7ECE88C647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D27C854-17B4-4C18-9F93-C767DED7D58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:I1012"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1901,7 +1901,7 @@
         <v>44523</v>
       </c>
       <c r="H25" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="66"/>
     </row>
@@ -1926,7 +1926,7 @@
         <v>44523</v>
       </c>
       <c r="H26" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="66"/>
     </row>
@@ -1951,7 +1951,7 @@
         <v>44523</v>
       </c>
       <c r="H27" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="66"/>
     </row>
@@ -1976,7 +1976,7 @@
         <v>44523</v>
       </c>
       <c r="H28" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="66"/>
     </row>

</xml_diff>

<commit_message>
Actualizacion Porcentaje de Avance del Proyecto - Sprint 2
</commit_message>
<xml_diff>
--- a/Desarrollo/MP/Gestión/MP-CP.xlsx
+++ b/Desarrollo/MP/Gestión/MP-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUZ ELENA\Documents\GitHub\Orangesoft\Desarrollo\MP\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D27C854-17B4-4C18-9F93-C767DED7D58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132BED0A-7FA0-4E24-A293-613FE1F2A70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1355,8 +1355,8 @@
   </sheetPr>
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2001,7 +2001,7 @@
         <v>44524</v>
       </c>
       <c r="H29" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="65" t="s">
         <v>79</v>
@@ -2028,7 +2028,7 @@
         <v>44524</v>
       </c>
       <c r="H30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="66"/>
     </row>
@@ -2047,7 +2047,7 @@
         <v>44524</v>
       </c>
       <c r="H31" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="66"/>
     </row>

</xml_diff>

<commit_message>
Actualizar Porcentaje de Avance Hito N°3
Actualizar Porcentaje de Avance Hito N°3
</commit_message>
<xml_diff>
--- a/Desarrollo/MP/Gestión/MP-CP.xlsx
+++ b/Desarrollo/MP/Gestión/MP-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUZ ELENA\Documents\GitHub\Orangesoft\Desarrollo\MP\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132BED0A-7FA0-4E24-A293-613FE1F2A70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43917653-859D-478A-9785-34C75454504E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1355,8 +1355,8 @@
   </sheetPr>
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2069,10 +2069,10 @@
         <v>44524</v>
       </c>
       <c r="G32" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H32" s="23">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I32" s="65" t="s">
         <v>85</v>
@@ -2096,10 +2096,10 @@
         <v>44524</v>
       </c>
       <c r="G33" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H33" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="66"/>
     </row>
@@ -2121,10 +2121,10 @@
         <v>44524</v>
       </c>
       <c r="G34" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H34" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="66"/>
     </row>
@@ -2146,10 +2146,10 @@
         <v>44524</v>
       </c>
       <c r="G35" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H35" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="66"/>
     </row>
@@ -2171,10 +2171,10 @@
         <v>44524</v>
       </c>
       <c r="G36" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H36" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="66"/>
     </row>
@@ -2196,7 +2196,7 @@
         <v>44531</v>
       </c>
       <c r="G37" s="22">
-        <v>44545</v>
+        <v>44550</v>
       </c>
       <c r="H37" s="23">
         <v>0</v>
@@ -2221,10 +2221,10 @@
         <v>44543</v>
       </c>
       <c r="G38" s="22">
-        <v>44545</v>
+        <v>44550</v>
       </c>
       <c r="H38" s="23">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I38" s="65" t="s">
         <v>99</v>
@@ -2248,7 +2248,7 @@
         <v>44543</v>
       </c>
       <c r="G39" s="22">
-        <v>44545</v>
+        <v>44550</v>
       </c>
       <c r="H39" s="23">
         <v>0</v>

</xml_diff>

<commit_message>
Actualización Porcentaje de Avance H3
Actualización Porcentaje de Avance H3
</commit_message>
<xml_diff>
--- a/Desarrollo/MP/Gestión/MP-CP.xlsx
+++ b/Desarrollo/MP/Gestión/MP-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUZ ELENA\Documents\GitHub\Orangesoft\Desarrollo\MP\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132BED0A-7FA0-4E24-A293-613FE1F2A70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E27550-89B5-4C1E-93CD-E7BFAC5357F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1355,8 +1355,8 @@
   </sheetPr>
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2069,10 +2069,10 @@
         <v>44524</v>
       </c>
       <c r="G32" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H32" s="23">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I32" s="65" t="s">
         <v>85</v>
@@ -2096,10 +2096,10 @@
         <v>44524</v>
       </c>
       <c r="G33" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H33" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="66"/>
     </row>
@@ -2121,10 +2121,10 @@
         <v>44524</v>
       </c>
       <c r="G34" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H34" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="66"/>
     </row>
@@ -2146,10 +2146,10 @@
         <v>44524</v>
       </c>
       <c r="G35" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H35" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="66"/>
     </row>
@@ -2171,10 +2171,10 @@
         <v>44524</v>
       </c>
       <c r="G36" s="22">
-        <v>44542</v>
+        <v>44550</v>
       </c>
       <c r="H36" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="66"/>
     </row>
@@ -2196,7 +2196,7 @@
         <v>44531</v>
       </c>
       <c r="G37" s="22">
-        <v>44545</v>
+        <v>44550</v>
       </c>
       <c r="H37" s="23">
         <v>0</v>
@@ -2221,7 +2221,7 @@
         <v>44543</v>
       </c>
       <c r="G38" s="22">
-        <v>44545</v>
+        <v>44550</v>
       </c>
       <c r="H38" s="23">
         <v>0</v>
@@ -2248,7 +2248,7 @@
         <v>44543</v>
       </c>
       <c r="G39" s="22">
-        <v>44545</v>
+        <v>44550</v>
       </c>
       <c r="H39" s="23">
         <v>0</v>

</xml_diff>

<commit_message>
Actualizacion porcentaje de avance final del proyecto
Actualizacion porcentaje de avance final del proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/MP/Gestión/MP-CP.xlsx
+++ b/Desarrollo/MP/Gestión/MP-CP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUZ ELENA\Documents\GitHub\Orangesoft\Desarrollo\MP\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C01816-019A-4C28-ADAE-3D42F3866292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5423633C-A39B-4B1B-8A2A-6978B58A6C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3945" yWindow="540" windowWidth="9090" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
@@ -1093,6 +1093,12 @@
     <xf numFmtId="165" fontId="15" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="15" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1104,12 +1110,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1370,7 +1370,7 @@
   </sheetPr>
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
@@ -1387,23 +1387,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
     </row>
     <row r="2" spans="1:9" ht="12.75">
       <c r="A2" s="1"/>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="61"/>
+      <c r="C2" s="63"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1562,7 +1562,7 @@
       <c r="H11" s="40">
         <v>1</v>
       </c>
-      <c r="I11" s="57" t="s">
+      <c r="I11" s="59" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1589,7 +1589,7 @@
       <c r="H12" s="40">
         <v>1</v>
       </c>
-      <c r="I12" s="58"/>
+      <c r="I12" s="60"/>
     </row>
     <row r="13" spans="1:9" ht="12.75">
       <c r="A13" s="11"/>
@@ -1614,7 +1614,7 @@
       <c r="H13" s="40">
         <v>1</v>
       </c>
-      <c r="I13" s="57" t="s">
+      <c r="I13" s="59" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       <c r="H14" s="40">
         <v>1</v>
       </c>
-      <c r="I14" s="58"/>
+      <c r="I14" s="60"/>
     </row>
     <row r="15" spans="1:9" ht="12.75">
       <c r="A15" s="11"/>
@@ -1666,7 +1666,7 @@
       <c r="H15" s="40">
         <v>1</v>
       </c>
-      <c r="I15" s="58"/>
+      <c r="I15" s="60"/>
     </row>
     <row r="16" spans="1:9" ht="12.75">
       <c r="A16" s="11"/>
@@ -1691,7 +1691,7 @@
       <c r="H16" s="40">
         <v>1</v>
       </c>
-      <c r="I16" s="58"/>
+      <c r="I16" s="60"/>
     </row>
     <row r="17" spans="1:9" ht="12.75">
       <c r="A17" s="11"/>
@@ -1716,7 +1716,7 @@
       <c r="H17" s="40">
         <v>1</v>
       </c>
-      <c r="I17" s="57" t="s">
+      <c r="I17" s="59" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1743,7 +1743,7 @@
       <c r="H18" s="40">
         <v>1</v>
       </c>
-      <c r="I18" s="58"/>
+      <c r="I18" s="60"/>
     </row>
     <row r="19" spans="1:9" ht="12.75">
       <c r="A19" s="11"/>
@@ -1768,7 +1768,7 @@
       <c r="H19" s="40">
         <v>1</v>
       </c>
-      <c r="I19" s="58"/>
+      <c r="I19" s="60"/>
     </row>
     <row r="20" spans="1:9" ht="12.75">
       <c r="A20" s="11"/>
@@ -1820,7 +1820,7 @@
       <c r="H21" s="40">
         <v>1</v>
       </c>
-      <c r="I21" s="57" t="s">
+      <c r="I21" s="59" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1847,7 +1847,7 @@
       <c r="H22" s="40">
         <v>1</v>
       </c>
-      <c r="I22" s="58"/>
+      <c r="I22" s="60"/>
     </row>
     <row r="23" spans="1:9" ht="12.75">
       <c r="A23" s="11"/>
@@ -1866,7 +1866,7 @@
       <c r="H23" s="43">
         <v>1</v>
       </c>
-      <c r="I23" s="58"/>
+      <c r="I23" s="60"/>
     </row>
     <row r="24" spans="1:9" ht="12.75">
       <c r="A24" s="11"/>
@@ -1891,7 +1891,7 @@
       <c r="H24" s="45">
         <v>1</v>
       </c>
-      <c r="I24" s="57" t="s">
+      <c r="I24" s="59" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1918,7 +1918,7 @@
       <c r="H25" s="46">
         <v>1</v>
       </c>
-      <c r="I25" s="58"/>
+      <c r="I25" s="60"/>
     </row>
     <row r="26" spans="1:9" ht="12.75">
       <c r="A26" s="11"/>
@@ -1943,7 +1943,7 @@
       <c r="H26" s="45">
         <v>1</v>
       </c>
-      <c r="I26" s="58"/>
+      <c r="I26" s="60"/>
     </row>
     <row r="27" spans="1:9" ht="12.75">
       <c r="A27" s="11"/>
@@ -1968,7 +1968,7 @@
       <c r="H27" s="46">
         <v>1</v>
       </c>
-      <c r="I27" s="58"/>
+      <c r="I27" s="60"/>
     </row>
     <row r="28" spans="1:9" ht="12.75">
       <c r="A28" s="11"/>
@@ -1993,7 +1993,7 @@
       <c r="H28" s="40">
         <v>1</v>
       </c>
-      <c r="I28" s="58"/>
+      <c r="I28" s="60"/>
     </row>
     <row r="29" spans="1:9" ht="12.75">
       <c r="A29" s="11"/>
@@ -2018,7 +2018,7 @@
       <c r="H29" s="40">
         <v>1</v>
       </c>
-      <c r="I29" s="57" t="s">
+      <c r="I29" s="59" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       <c r="H30" s="40">
         <v>1</v>
       </c>
-      <c r="I30" s="58"/>
+      <c r="I30" s="60"/>
     </row>
     <row r="31" spans="1:9" ht="12.75">
       <c r="A31" s="11"/>
@@ -2053,8 +2053,8 @@
         <v>76</v>
       </c>
       <c r="C31" s="19"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
       <c r="F31" s="21">
         <v>44510</v>
       </c>
@@ -2064,7 +2064,7 @@
       <c r="H31" s="43">
         <v>1</v>
       </c>
-      <c r="I31" s="58"/>
+      <c r="I31" s="60"/>
     </row>
     <row r="32" spans="1:9" ht="12.75">
       <c r="A32" s="11"/>
@@ -2089,7 +2089,7 @@
       <c r="H32" s="40">
         <v>1</v>
       </c>
-      <c r="I32" s="57" t="s">
+      <c r="I32" s="59" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
       <c r="H33" s="40">
         <v>1</v>
       </c>
-      <c r="I33" s="58"/>
+      <c r="I33" s="60"/>
     </row>
     <row r="34" spans="1:9" ht="12.75">
       <c r="A34" s="11"/>
@@ -2141,7 +2141,7 @@
       <c r="H34" s="40">
         <v>1</v>
       </c>
-      <c r="I34" s="58"/>
+      <c r="I34" s="60"/>
     </row>
     <row r="35" spans="1:9" ht="12.75">
       <c r="A35" s="11"/>
@@ -2166,7 +2166,7 @@
       <c r="H35" s="40">
         <v>1</v>
       </c>
-      <c r="I35" s="58"/>
+      <c r="I35" s="60"/>
     </row>
     <row r="36" spans="1:9" ht="12.75">
       <c r="A36" s="11"/>
@@ -2191,7 +2191,7 @@
       <c r="H36" s="40">
         <v>1</v>
       </c>
-      <c r="I36" s="58"/>
+      <c r="I36" s="60"/>
     </row>
     <row r="37" spans="1:9" ht="14.25" customHeight="1">
       <c r="A37" s="11"/>
@@ -2216,7 +2216,7 @@
       <c r="H37" s="40">
         <v>1</v>
       </c>
-      <c r="I37" s="58"/>
+      <c r="I37" s="60"/>
     </row>
     <row r="38" spans="1:9" ht="12.75">
       <c r="A38" s="11"/>
@@ -2241,7 +2241,7 @@
       <c r="H38" s="40">
         <v>1</v>
       </c>
-      <c r="I38" s="57" t="s">
+      <c r="I38" s="59" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2268,7 +2268,7 @@
       <c r="H39" s="40">
         <v>1</v>
       </c>
-      <c r="I39" s="58"/>
+      <c r="I39" s="60"/>
     </row>
     <row r="40" spans="1:9" ht="12.75">
       <c r="A40" s="11"/>
@@ -2293,7 +2293,7 @@
       <c r="H40" s="40">
         <v>1</v>
       </c>
-      <c r="I40" s="57" t="s">
+      <c r="I40" s="59" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2320,7 +2320,7 @@
       <c r="H41" s="40">
         <v>1</v>
       </c>
-      <c r="I41" s="58"/>
+      <c r="I41" s="60"/>
     </row>
     <row r="42" spans="1:9" ht="12.75">
       <c r="A42" s="11"/>
@@ -2345,7 +2345,7 @@
       <c r="H42" s="40">
         <v>1</v>
       </c>
-      <c r="I42" s="58"/>
+      <c r="I42" s="60"/>
     </row>
     <row r="43" spans="1:9" ht="12.75">
       <c r="B43" s="51" t="s">
@@ -2383,7 +2383,7 @@
       <c r="G44" s="56">
         <v>44550</v>
       </c>
-      <c r="H44" s="63">
+      <c r="H44" s="57">
         <v>1</v>
       </c>
     </row>
@@ -7271,10 +7271,10 @@
       <c r="C2" s="24"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="64" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="61"/>
+      <c r="C3" s="63"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
       <c r="B4" s="25" t="s">

</xml_diff>